<commit_message>
changes made to gui_version_2
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,16 @@
           <t>Media</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Channel</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-10-09 11:41:32</t>
+          <t>2024-10-09 19:22:36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -474,17 +479,18 @@
       <c r="C2" t="n">
         <v>13052054965</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Hi</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-10-09_23-22-36.jpg</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-10-09 11:41:57</t>
+          <t>2024-10-13 17:48:26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -497,19 +503,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>media_files\photo_2024-10-09_15-41-56.jpg</t>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>new_channel'</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-10-09 11:47:39</t>
+          <t>2024-10-13 17:54:46</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -526,11 +533,16 @@
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>new_channel'</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-10-09 11:48:25</t>
+          <t>2024-10-13 23:49:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -543,15 +555,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hi</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-10-14_03-48-59.jpg</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-10-09 11:53:29</t>
+          <t>2024-10-14 19:10:34</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -564,15 +581,20 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hi</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-10-14_23-10-33.jpg</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-10-09 12:39:14</t>
+          <t>2024-10-14 19:11:09</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -585,15 +607,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Hi</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-10-14_23-11-07.jpg</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-10-09 12:41:19</t>
+          <t>2024-10-14 19:19:39</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -606,15 +633,20 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Hi</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-10-14_23-19-38.jpg</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-10-09 12:41:37</t>
+          <t>2024-10-14 19:22:55</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -622,151 +654,22 @@
           <t>nnn222111</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>13052054965</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hi</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-10-09 12:41:55</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>nnn222111</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>13052054965</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Hello</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-10-09 12:42:14</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>nnn222111</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>13052054965</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-10-09 12:49:54</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>nnn222111</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>13052054965</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
           <t>Test 2</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-10-09 12:50:08</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>nnn222111</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>13052054965</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Test 3</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-10-09 12:50:26</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nnn222111</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>13052054965</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>media_files\photo_2024-10-09_16-50-25.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-10-09 18:22:49</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>nnn222111</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>13052054965</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>media_files\photo_2024-10-09_22-22-48.jpg</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-10-14_23-22-54.jpg</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completing of python side of app
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -654,22 +654,66 @@
           <t>nnn222111</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-10-14_23-22-54.jpg</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-12-02 21:21:50</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-12-02 21:22:33</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>13052054965</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Test 2</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>media_files\photo_2024-10-14_23-22-54.jpg</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
addition of upload handler and io socket for images in index.html
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,10 +702,8 @@
           <t>nnn222111</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>13052054965</t>
-        </is>
+      <c r="C11" t="n">
+        <v>13052054965</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -714,6 +712,628 @@
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:18:38</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-18-38.jpg</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:19:47</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-19-47.jpg</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:20:30</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-20-30.jpg</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:21:03</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-21-03.jpg</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:27:43</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-27-44.jpg</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:30:36</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-30-36.jpg</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:35:14</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-35-14.jpg</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:37:00</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-37-00.jpg</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:47:10</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-47-11.jpg</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:47:55</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-47-55.jpg</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:48:58</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-48-58.jpg</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:50:23</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:56:55</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-56-55.jpg</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-12-03 21:58:16</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_02-58-16.jpg</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:02:00</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-02-00.jpg</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:03:10</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-03-11.jpg</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:04:18</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-04-19.jpg</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:04:45</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-04-45.jpg</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:06:39</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-06-39.jpg</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:07:15</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-07-15.jpg</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:08:49</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-08-50.jpg</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:11:11</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-11-12.jpg</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:12:17</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>13052054965</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-12-18.jpg</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-12-03 22:12:36</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>nnn222111</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>media_files\photo_2024-12-04_03-12-37.jpg</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
starting to incorporate a mysql db in this project
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,6 +626,141 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-09-19 20:35:14</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-09-19 21:03:51</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-09-19 21:10:32</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-09-19 21:11:51</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-09-19 21:12:13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Yo</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
creation of post and get routes for the server. post request implemented in index.html for text messages. Next task: allow route to handle media; change messages table to add media options
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,6 +761,114 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-09-21 14:24:59</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-09-21 15:40:12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-09-21 16:03:15</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-09-21 16:04:02</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
completion of backend routes, such as get requests and post requests. Ready to start front end development
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,6 +869,502 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-09-23 12:49:42</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>media_files\photo_2025-09-23_16-49-42.jpg</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-09-23 15:05:59</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>media_files\photo_2025-09-23_19-05-59.jpg</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-09-23 15:07:25</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Hiii</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>my-node-server/uploads/images\photo_2025-09-23_19-07-25.jpg</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-09-23 15:20:01</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>my-node-server/uploads/images\photo_2025-09-23_19-20-01.jpg</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-09-23 15:30:16</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Whats up</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>my-node-server/uploads/images\photo_2025-09-23_19-30-16.jpg</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-09-23 15:40:39</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Yo</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-23_19-40-39.jpg</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-09-23 15:43:25</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Hey</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-23_19-43-25.jpg</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-09-23 15:43:45</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Yuh</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-23_19-43-45.jpg</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-09-23 15:58:02</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/videos\video.mp4</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-09-23 20:30:25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Yooooo</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-24_00-30-25.jpg</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-09-23 20:35:42</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-24_00-35-42.jpg</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-09-23 20:43:43</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-24_00-43-43.jpg</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-09-23 20:44:46</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-24_00-44-46.jpg</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-09-23 20:48:08</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>What’s up man</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-24_00-48-08.jpg</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-09-23 20:54:17</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Hey</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-24_00-54-17.jpg</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-09-23 20:57:01</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>What’s up man</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-09-24_00-57-02.jpg</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new messages show up now in real time; error shows in console when images are sent in real time
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1365,6 +1365,280 @@
       </c>
       <c r="G32" t="inlineStr"/>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-10-02 14:11:48</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Hey man what’s up?</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-10-02 14:41:25</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-10-02 14:43:50</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-10-02 14:44:07</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>What’s up man?</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-10-02 14:45:00</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-10-02 14:50:33</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Test messages</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-10-02 14:51:56</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Yo</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-10-02 15:39:53</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-10-02 15:41:27</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Test messages</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-10-02 15:42:18</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-10-02_19-42-18.jpg</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
full implementation of socket io to sender.htm. next task: implement socket io to index.html to show new senders and channels
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1639,6 +1639,373 @@
       </c>
       <c r="G42" t="inlineStr"/>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-10-02 20:29:18</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-10-03_00-29-18.jpg</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-10-02 20:34:00</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-10-03_00-34-01.jpg</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-10-02 20:34:46</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-10-02 20:38:35</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-10-02 20:40:25</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>What’s up?</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-10-02 20:40:44</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-10-03_00-40-45.jpg</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-10-02 20:51:16</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-10-02 21:09:20</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-10-03_01-09-20.jpg</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-10-02 21:10:27</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-10-02 21:11:06</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Latest message</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-10-02 21:11:17</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Message again</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-10-02 21:12:37</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-10-02 21:13:09</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Test 113</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added padding bottom to messages
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2006,6 +2006,37 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-10-02 21:24:40</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-10-03_01-24-41.jpg</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updates new senders to index.html in real time. New route added to get senders by enternal id
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2037,6 +2037,195 @@
       </c>
       <c r="G56" t="inlineStr"/>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-10-04 18:55:06</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Hey man what’s up?</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-10-04 18:56:34</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Hey man what’s up?</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-10-04 19:25:39</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Hey man what’s up?</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-10-04 19:27:47</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Hey man what’s up?</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-10-04 19:29:36</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-10-04 19:30:42</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-10-04 19:31:22</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chnages caused by data being saved from messages
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2226,6 +2226,168 @@
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-10-12 16:11:21</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Hey man what’s up?</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-10-12 16:11:48</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>How is your day going?</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-10-12 16:12:08</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>What are you doing today?</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-10-12 16:12:22</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-10-12 16:15:58</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>One more test message</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-10-12 16:16:11</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>And another</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
http post request is now being sent from main.py and not server.js. timestamp type checking was removed from messages.post.js because Date(timestamp) was giving inaccurate times.
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2388,6 +2388,114 @@
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-10-14 20:32:37</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-10-14 20:45:23</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-10-14 20:47:27</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>This message was sent at 8:47 pm</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-10-14 20:54:13</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>This message was sent at 8:54 pm</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed issue with displaying and storing the correct date
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2496,6 +2496,276 @@
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-10-18 09:15:30</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-10-18 09:16:44</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-10-18 09:19:57</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-10-18 09:23:22</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-10-18 09:25:43</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-10-18 09:40:59</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-10-18 09:43:28</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>This message was sent at 9:43 am</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-10-18 09:45:59</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>This message was sent at 9:45 am</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-10-18 10:15:53</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>This message was sent at 10:15 am</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-10-18 10:18:15</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>This message was sent at 10:18 am</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
main.py - channels can now be passed to the post request messages.get.js - channels messages can be returned even if sender id is null messages.post.js - channel messages can be posted even when sender id is null
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2766,6 +2766,462 @@
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-10-20 18:33:13</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-10-20 18:34:36</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-10-20 18:35:28</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-10-20 18:35:43</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-10-20 18:42:13</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Hey guys</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-10-20 18:45:23</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:00:08</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:01:49</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:02:54</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:08:35</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:08:35</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Test message</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:09:30</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:10:11</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:10:32</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-10-20 19:12:10</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-10-20 20:25:40</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Noahs channel</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
changed main.py to add back save_message function in line 147
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3222,6 +3222,37 @@
         </is>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-10-22 21:10:29</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>My floor</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>my-node-server/public/uploads/images\photo_2025-10-23_01-10-29.jpg</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
timestamp change to nyc time
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3525,6 +3525,60 @@
         </is>
       </c>
     </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-10-26 02:30:05</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-10-25 22:45:50</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>10:45</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
tested version of sender and channel filtering
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3579,6 +3579,114 @@
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
     </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-12-31 21:49:08</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-12-31 21:52:08</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-12-31 21:55:08</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Hey man</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-12-31 22:24:00</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
changes to the debugging console output + no longer saves messages to excel
</commit_message>
<xml_diff>
--- a/conversations_with_media.xlsx
+++ b/conversations_with_media.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3849,6 +3849,311 @@
       <c r="F122" t="inlineStr"/>
       <c r="G122" t="inlineStr"/>
     </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:06:32</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:36:50</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:37:37</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:37:44</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2026-01-09 21:30:01</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Noahs life</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Noahs life</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:38:50</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Noahs life</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Noahs life</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:40:05</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Noah Dubitzky</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>8450689526</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>13052054965</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Idk</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:40:52</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Emerson Walker</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>8483444103</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>My name is Emerson and its a please to talk to you.</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:41:22</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Emerson Walker</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>8483444103</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>I’d like to take a moment to explain the purpose of my outreach.</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr"/>
+      <c r="G131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:38:50</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Noahs life</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr"/>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Noahs life</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2026-01-10 20:45:44</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Noahs life</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr"/>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>Noahs life</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>